<commit_message>
feat(assets): fill with some data
</commit_message>
<xml_diff>
--- a/assets/prices_log.xlsx
+++ b/assets/prices_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMarian\Desktop\API Testing\price-scrap\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19A0C47-0897-4186-A544-9676CDA5F66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FEC3B3-921A-4612-9872-49E093B0DDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Product</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>155,00 Lei</t>
+  </si>
+  <si>
+    <t>35,05 Lei</t>
+  </si>
+  <si>
+    <t>31,40 Lei</t>
+  </si>
+  <si>
+    <t>108,00 Lei</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,17 +365,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
@@ -370,7 +389,42 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45503.762067337957</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45503.762077187501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45503.762085902781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45503.762094070808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(emag-product-page: function name changed
</commit_message>
<xml_diff>
--- a/assets/prices_log.xlsx
+++ b/assets/prices_log.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMarian\Desktop\API Testing\price-scrap\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32FEC3B3-921A-4612-9872-49E093B0DDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF75F6E-55F0-4E0A-AF49-FD543BDC0DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Base-Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Product</t>
   </si>
@@ -28,22 +28,31 @@
     <t>Price</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Cafea Organica House Roast, Exhale, boabe</t>
   </si>
   <si>
     <t>155,00 Lei</t>
   </si>
   <si>
+    <t>Klorane Urzica Sampon uscat 150 ml</t>
+  </si>
+  <si>
     <t>35,05 Lei</t>
   </si>
   <si>
+    <t>Crema pentru ochi Elmiplant Hyaluronic Gold, Femei, 15 ml</t>
+  </si>
+  <si>
     <t>31,40 Lei</t>
   </si>
   <si>
+    <t>Bautura de Ovaz Standard Minor Figures bax 6L</t>
+  </si>
+  <si>
     <t>108,00 Lei</t>
-  </si>
-  <si>
-    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -53,8 +62,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,9 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,66 +385,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45504.042433495371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45504.042444629631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45504.042452569447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45504.042459872682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
-        <v>45503.762067337957</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>45503.762077187501</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C6" s="1">
+        <v>45504.044278368063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
-        <v>45503.762085902781</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
-        <v>45503.762094070808</v>
+      <c r="C7" s="1">
+        <v>45504.044287997684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45504.044296539352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45504.044303949639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(offer-problem): added an additional check when checking the price, if there are a small number of offers on the product.
</commit_message>
<xml_diff>
--- a/assets/prices_log.xlsx
+++ b/assets/prices_log.xlsx
@@ -406,7 +406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -973,7 +973,337 @@
         </is>
       </c>
       <c r="C37" s="3" t="n">
-        <v>45504.05657502977</v>
+        <v>45504.05657503472</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Cafea Organica House Roast, Exhale, boabe</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>155,00 Lei</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>45504.06547949074</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Klorane Urzica Sampon uscat 150 ml</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>35,05 Lei</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>45504.06548925926</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Crema pentru ochi Elmiplant Hyaluronic Gold, Femei, 15 ml</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>31,40 Lei</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>45504.06549770833</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Bautura de Ovaz Standard Minor Figures bax 6L</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>108,00 Lei</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>45504.06550571759</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Cafea Organica House Roast, Exhale, boabe</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>155,00 Lei</t>
+        </is>
+      </c>
+      <c r="C42" s="3" t="n">
+        <v>45504.06703585648</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Klorane Urzica Sampon uscat 150 ml</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>35,05 Lei</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>45504.06704974537</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Crema pentru ochi Elmiplant Hyaluronic Gold, Femei, 15 ml</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>31,40 Lei</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>45504.0670582176</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Bautura de Ovaz Standard Minor Figures bax 6L</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>108,00 Lei</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>45504.06706739583</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Cafea Organica House Roast, Exhale, boabe</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>155,00 Lei</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>45504.06756972223</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Klorane Urzica Sampon uscat 150 ml</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>35,05 Lei</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="n">
+        <v>45504.06757984954</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Crema pentru ochi Elmiplant Hyaluronic Gold, Femei, 15 ml</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>31,40 Lei</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="n">
+        <v>45504.06759200231</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Bautura de Ovaz Standard Minor Figures bax 6L</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>108,00 Lei</t>
+        </is>
+      </c>
+      <c r="C49" s="3" t="n">
+        <v>45504.06759958333</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Cafea Organica House Roast, Exhale, boabe</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>155,00 Lei</t>
+        </is>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>45504.06967789352</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Klorane Urzica Sampon uscat 150 ml</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>35,05 Lei</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>45504.06968862269</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Crema pentru ochi Elmiplant Hyaluronic Gold, Femei, 15 ml</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>31,40 Lei</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="n">
+        <v>45504.06969699074</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Bautura de Ovaz Standard Minor Figures bax 6L</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>108,00 Lei</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>45504.06970663195</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Prelata acoperire piscina, PVC, neagra, 366 cm, Bestway</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>149,80 Lei</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>45504.06972070602</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Cafea Organica House Roast, Exhale, boabe</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>155,00 Lei</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>45504.07166885417</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Klorane Urzica Sampon uscat 150 ml</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>35,05 Lei</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>45504.07167846065</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Crema pentru ochi Elmiplant Hyaluronic Gold, Femei, 15 ml</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>31,40 Lei</t>
+        </is>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>45504.07168659722</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Bautura de Ovaz Standard Minor Figures bax 6L</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>108,00 Lei</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>45504.07169497685</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Prelata acoperire piscina, PVC, neagra, 366 cm, Bestway</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>149,80 Lei</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>45504.07170875659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>